<commit_message>
commiting on 17 Aug 1:33 AM
</commit_message>
<xml_diff>
--- a/Iceberg_Work_Done.xlsx
+++ b/Iceberg_Work_Done.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anshumanr/Documents/Iceberg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFBA978-F013-8447-A0B0-FA51F527FA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E0AB65-59F1-C74F-B345-0CAE54AA9D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15780" xr2:uid="{87869312-4B3D-5545-9FC6-72200158867B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{87869312-4B3D-5545-9FC6-72200158867B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>TOPICS</t>
   </si>
@@ -56,7 +56,19 @@
     <t>Transactions in Iceberg table</t>
   </si>
   <si>
-    <t>Doing</t>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>Update a record will create a new data file and the original file will be kept as it is. Original file size : 1 KB and After modifying file size : 2KB</t>
+  </si>
+  <si>
+    <t>Deleting records where class_year &lt; 2020. It deleted all the records from year 2019. No records from 2019 are shown in the table, but the data file containing all records from 2019 is present. It will be used to see the historic data.</t>
+  </si>
+  <si>
+    <t>COW table</t>
+  </si>
+  <si>
+    <t>Upserting data from new_table to students</t>
   </si>
 </sst>
 </file>
@@ -111,11 +123,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,63 +451,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E17E8A1-3129-1448-B7B2-166907455839}">
-  <dimension ref="A1:B460"/>
+  <dimension ref="A1:C460"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.5" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="2" width="47.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="32.5" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:2" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="3" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="17" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="18" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="19" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
@@ -932,6 +978,10 @@
     <row r="459" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="460" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:C7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commiting at 17 aug 2023 3:20 PM
</commit_message>
<xml_diff>
--- a/Iceberg_Work_Done.xlsx
+++ b/Iceberg_Work_Done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anshumanr/Documents/Iceberg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E0AB65-59F1-C74F-B345-0CAE54AA9D2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3732C4-EA3E-4C41-9AD1-C723A30A4305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{87869312-4B3D-5545-9FC6-72200158867B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>TOPICS</t>
   </si>
@@ -69,13 +69,25 @@
   </si>
   <si>
     <t>Upserting data from new_table to students</t>
+  </si>
+  <si>
+    <t>Doing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOR Table (Applicable for Format-version : 2 only) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Update a record will create two new files, a file which contains file path of the previous file and the position of the record in the table which is to be deleted (or deleted for updating the table) , and the second file which only contains the updated record.</t>
+  </si>
+  <si>
+    <t>The format-version property in an Apache Iceberg table specifies the version of the Iceberg table format that the table uses. The current version of the Iceberg table format is 2. Version 1 of the Iceberg table format does not support row-level deletes.  Version 2 of the Iceberg table format adds support for row-level deletes. This means that you can delete or replace individual rows in immutable data files without rewriting the files.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,6 +114,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -123,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -132,10 +150,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,20 +475,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E17E8A1-3129-1448-B7B2-166907455839}">
-  <dimension ref="A1:C460"/>
+  <dimension ref="A1:D460"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="47.1640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="55.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="58.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.5" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="79.5" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -483,7 +509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -491,7 +517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -499,40 +525,59 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:4" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" ht="100" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:3" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" s="3" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="17" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="18" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="19" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
@@ -978,9 +1023,11 @@
     <row r="459" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="460" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="C5:C7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Commiting at 18 Aug 2023 7:10 PM
</commit_message>
<xml_diff>
--- a/Iceberg_Work_Done.xlsx
+++ b/Iceberg_Work_Done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anshumanr/Documents/Iceberg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3732C4-EA3E-4C41-9AD1-C723A30A4305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9DB3FC-7D56-A04D-A28C-4891A66B0137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{87869312-4B3D-5545-9FC6-72200158867B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>TOPICS</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Upserting data from new_table to students</t>
   </si>
   <si>
-    <t>Doing</t>
-  </si>
-  <si>
     <t xml:space="preserve">MOR Table (Applicable for Format-version : 2 only) </t>
   </si>
   <si>
@@ -81,6 +78,47 @@
   </si>
   <si>
     <t>The format-version property in an Apache Iceberg table specifies the version of the Iceberg table format that the table uses. The current version of the Iceberg table format is 2. Version 1 of the Iceberg table format does not support row-level deletes.  Version 2 of the Iceberg table format adds support for row-level deletes. This means that you can delete or replace individual rows in immutable data files without rewriting the files.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upserting data from new_table to students. It deleted the records and then create a new record coming from new_table </t>
+  </si>
+  <si>
+    <t>Table Properties</t>
+  </si>
+  <si>
+    <t>parquet vectorization</t>
+  </si>
+  <si>
+    <t>Sub-topics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default parquet vectorization will be turned on in version 1.3.1. This changes the behavior of how data is delivered from one row at a time to column batches which can improve performance. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write format </t>
+  </si>
+  <si>
+    <t>write.format.default = parquet or avro or orc</t>
+  </si>
+  <si>
+    <t>Compression format</t>
+  </si>
+  <si>
+    <t>write.parquet.compression-codec = zstd, brotli, lz4, gzip, snappy, uncompressed. Bydefault = gzip</t>
+  </si>
+  <si>
+    <t>cleaning up metadata files</t>
+  </si>
+  <si>
+    <t>set a limit on how many are retained so older ones are cleaned up using properties: 'write.metadata.delete-after-commit.enabled'='true' , 'write.metadata.previous-versions-max'=50,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Object storage compability </t>
+  </si>
+  <si>
+    <t>If a table has many columns, tracking the metrics for all columns can get very expensive to your writes. You can manage metrics and turn them off for columns where they may not be relevant to your query patterns. 
+'write.object-storage.enabled'=true,
+'write.data.path'='s3://my-path-data-bucket'</t>
   </si>
 </sst>
 </file>
@@ -141,13 +179,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -160,6 +201,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,109 +522,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E17E8A1-3129-1448-B7B2-166907455839}">
-  <dimension ref="A1:D460"/>
+  <dimension ref="A1:E460"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="104" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="58.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="32.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="79.5" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="2" width="55.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="58.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="79.5" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5" t="s">
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" ht="100" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="100" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="8" t="s">
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" s="3" customFormat="1" ht="40" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="17" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="18" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="19" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
@@ -1023,11 +1134,13 @@
     <row r="459" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
     <row r="460" s="3" customFormat="1" ht="19" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="A11:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>